<commit_message>
set error handle in Release mode
</commit_message>
<xml_diff>
--- a/hw2.xlsx
+++ b/hw2.xlsx
@@ -12,10 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
-    <sheet name="FSOLVER.BISECTION" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="3" r:id="rId1"/>
+    <sheet name="FSOLVER.BISECTION" sheetId="1" r:id="rId2"/>
+    <sheet name="FDFSOLVER.NEWTON" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>FSOLVER</t>
   </si>
@@ -53,12 +54,30 @@
   <si>
     <t>AiryAi(x)</t>
   </si>
+  <si>
+    <t>FDFSOLVER</t>
+  </si>
+  <si>
+    <t>Homework 2</t>
+  </si>
+  <si>
+    <t>Create sheets FDFSOLVER.SECANT and FDFSOLVER.STEFFENSON based on FDFSOLVER.NEWTON</t>
+  </si>
+  <si>
+    <t>Create sheets FSOLVER.BRENT and FSOLVER.FALSEPOS based on FSOLVER.BISECTION</t>
+  </si>
+  <si>
+    <t>Which root finding method is the slowest to converge?</t>
+  </si>
+  <si>
+    <t>Which root finding method is the fastest to converge?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,13 +85,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,11 +119,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,11 +406,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M16"/>
+  <dimension ref="B2:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -430,15 +505,15 @@
       </c>
       <c r="E3">
         <f>_xll.GSL.ROOT.FSOLVER(D3)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="F3">
         <f>_xll.GSL.ROOT.FSOLVER.SET(E3, _xll.XLL.FUNCTION.REGID(_xll.GSL.SF.AIRY.AI), B3, B4)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G3">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F3)</f>
-        <v>-2.5</v>
+        <v>-2.25</v>
       </c>
       <c r="H3">
         <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F3)</f>
@@ -450,7 +525,7 @@
       </c>
       <c r="J3">
         <f>_xll.GSL.SF.AIRY.AI(G3)</f>
-        <v>-0.11232506769296607</v>
+        <v>6.1598658777005204E-2</v>
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
@@ -463,7 +538,7 @@
       </c>
       <c r="F4">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F3)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G4">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F4)</f>
@@ -475,7 +550,7 @@
       </c>
       <c r="I4">
         <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F4)</f>
-        <v>-2</v>
+        <v>-2.25</v>
       </c>
       <c r="J4">
         <f>_xll.GSL.SF.AIRY.AI(G4)</f>
@@ -485,7 +560,7 @@
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F5">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F4)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G5">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F5)</f>
@@ -507,11 +582,11 @@
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F6">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F5)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G6">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F6)</f>
-        <v>-2.34375</v>
+        <v>-2.3125</v>
       </c>
       <c r="H6">
         <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F6)</f>
@@ -519,17 +594,17 @@
       </c>
       <c r="I6">
         <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F6)</f>
-        <v>-2.3125</v>
+        <v>-2.25</v>
       </c>
       <c r="J6">
         <f>_xll.GSL.SF.AIRY.AI(G6)</f>
-        <v>-3.9565957042589422E-3</v>
+        <v>1.7951630456546505E-2</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F7">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F6)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G7">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F7)</f>
@@ -551,11 +626,11 @@
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F8">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F7)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G8">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F8)</f>
-        <v>-2.3359375</v>
+        <v>-2.328125</v>
       </c>
       <c r="H8">
         <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F8)</f>
@@ -563,17 +638,17 @@
       </c>
       <c r="I8">
         <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F8)</f>
-        <v>-2.328125</v>
+        <v>-2.3125</v>
       </c>
       <c r="J8">
         <f>_xll.GSL.SF.AIRY.AI(G8)</f>
-        <v>1.5215619082013588E-3</v>
+        <v>6.9995030229603418E-3</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F9">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F8)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G9">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F9)</f>
@@ -595,15 +670,15 @@
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F10">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F9)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G10">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F10)</f>
-        <v>-2.337890625</v>
+        <v>-2.33984375</v>
       </c>
       <c r="H10">
         <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F10)</f>
-        <v>-2.33984375</v>
+        <v>-2.34375</v>
       </c>
       <c r="I10">
         <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F10)</f>
@@ -611,17 +686,17 @@
       </c>
       <c r="J10">
         <f>_xll.GSL.SF.AIRY.AI(G10)</f>
-        <v>1.5201230781339975E-4</v>
+        <v>-1.2175386465713397E-3</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F11">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F10)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G11">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F11)</f>
-        <v>-2.3388671875</v>
+        <v>-2.337890625</v>
       </c>
       <c r="H11">
         <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F11)</f>
@@ -633,13 +708,13 @@
       </c>
       <c r="J11">
         <f>_xll.GSL.SF.AIRY.AI(G11)</f>
-        <v>-5.3276376360154832E-4</v>
+        <v>1.5201230781339975E-4</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F12">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F11)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G12">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F12)</f>
@@ -647,7 +722,7 @@
       </c>
       <c r="H12">
         <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F12)</f>
-        <v>-2.3388671875</v>
+        <v>-2.33984375</v>
       </c>
       <c r="I12">
         <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F12)</f>
@@ -661,7 +736,7 @@
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F13">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F12)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G13">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F13)</f>
@@ -683,11 +758,11 @@
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F14">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F13)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G14">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F14)</f>
-        <v>-2.3380126953125</v>
+        <v>-2.338134765625</v>
       </c>
       <c r="H14">
         <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F14)</f>
@@ -699,13 +774,13 @@
       </c>
       <c r="J14">
         <f>_xll.GSL.SF.AIRY.AI(G14)</f>
-        <v>6.6415286107069643E-5</v>
+        <v>-1.9181737913101437E-5</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F15">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F14)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G15">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F15)</f>
@@ -717,7 +792,7 @@
       </c>
       <c r="I15">
         <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F15)</f>
-        <v>-2.337890625</v>
+        <v>-2.3380126953125</v>
       </c>
       <c r="J15">
         <f>_xll.GSL.SF.AIRY.AI(G15)</f>
@@ -727,11 +802,11 @@
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F16">
         <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F15)</f>
-        <v>3.4604039834940927E-266</v>
+        <v>7.5038813227727042E-212</v>
       </c>
       <c r="G16">
         <f>_xll.GSL.ROOT.FSOLVER.ROOT(F16)</f>
-        <v>-2.33807373046875</v>
+        <v>-2.338104248046875</v>
       </c>
       <c r="H16">
         <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F16)</f>
@@ -739,11 +814,953 @@
       </c>
       <c r="I16">
         <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F16)</f>
-        <v>-2.3380126953125</v>
+        <v>-2.33807373046875</v>
       </c>
       <c r="J16">
         <f>_xll.GSL.SF.AIRY.AI(G16)</f>
-        <v>2.3616774199914496E-5</v>
+        <v>2.2175181458820866E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F16)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G17">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F17)</f>
+        <v>-2.338104248046875</v>
+      </c>
+      <c r="H17">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F17)</f>
+        <v>-2.338134765625</v>
+      </c>
+      <c r="I17">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F17)</f>
+        <v>-2.338104248046875</v>
+      </c>
+      <c r="J17">
+        <f>_xll.GSL.SF.AIRY.AI(G17)</f>
+        <v>2.2175181458820866E-6</v>
+      </c>
+    </row>
+    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F17)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G18">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F18)</f>
+        <v>-2.3381118774414062</v>
+      </c>
+      <c r="H18">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F18)</f>
+        <v>-2.338134765625</v>
+      </c>
+      <c r="I18">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F18)</f>
+        <v>-2.338104248046875</v>
+      </c>
+      <c r="J18">
+        <f>_xll.GSL.SF.AIRY.AI(G18)</f>
+        <v>-3.1322958704134886E-6</v>
+      </c>
+    </row>
+    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F18)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G19">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F19)</f>
+        <v>-2.3381061553955078</v>
+      </c>
+      <c r="H19">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F19)</f>
+        <v>-2.3381195068359375</v>
+      </c>
+      <c r="I19">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F19)</f>
+        <v>-2.338104248046875</v>
+      </c>
+      <c r="J19">
+        <f>_xll.GSL.SF.AIRY.AI(G19)</f>
+        <v>8.8006464182060097E-7</v>
+      </c>
+    </row>
+    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F19)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G20">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F20)</f>
+        <v>-2.3381061553955078</v>
+      </c>
+      <c r="H20">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F20)</f>
+        <v>-2.3381080627441406</v>
+      </c>
+      <c r="I20">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F20)</f>
+        <v>-2.338104248046875</v>
+      </c>
+      <c r="J20">
+        <f>_xll.GSL.SF.AIRY.AI(G20)</f>
+        <v>8.8006464182060097E-7</v>
+      </c>
+    </row>
+    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F20)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G21">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F21)</f>
+        <v>-2.3381061553955078</v>
+      </c>
+      <c r="H21">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F21)</f>
+        <v>-2.3381080627441406</v>
+      </c>
+      <c r="I21">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F21)</f>
+        <v>-2.338104248046875</v>
+      </c>
+      <c r="J21">
+        <f>_xll.GSL.SF.AIRY.AI(G21)</f>
+        <v>8.8006464182060097E-7</v>
+      </c>
+    </row>
+    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F21)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G22">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F22)</f>
+        <v>-2.3381075859069824</v>
+      </c>
+      <c r="H22">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F22)</f>
+        <v>-2.3381080627441406</v>
+      </c>
+      <c r="I22">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F22)</f>
+        <v>-2.3381071090698242</v>
+      </c>
+      <c r="J22">
+        <f>_xll.GSL.SF.AIRY.AI(G22)</f>
+        <v>-1.2302548615456236E-7</v>
+      </c>
+    </row>
+    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F22)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G23">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F23)</f>
+        <v>-2.3381073474884033</v>
+      </c>
+      <c r="H23">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F23)</f>
+        <v>-2.3381075859069824</v>
+      </c>
+      <c r="I23">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F23)</f>
+        <v>-2.3381071090698242</v>
+      </c>
+      <c r="J23">
+        <f>_xll.GSL.SF.AIRY.AI(G23)</f>
+        <v>4.4156201846437307E-8</v>
+      </c>
+    </row>
+    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F23)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G24">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F24)</f>
+        <v>-2.3381073474884033</v>
+      </c>
+      <c r="H24">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F24)</f>
+        <v>-2.3381075859069824</v>
+      </c>
+      <c r="I24">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F24)</f>
+        <v>-2.3381071090698242</v>
+      </c>
+      <c r="J24">
+        <f>_xll.GSL.SF.AIRY.AI(G24)</f>
+        <v>4.4156201846437307E-8</v>
+      </c>
+    </row>
+    <row r="25" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F24)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G25">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F25)</f>
+        <v>-2.3381074070930481</v>
+      </c>
+      <c r="H25">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F25)</f>
+        <v>-2.3381075859069824</v>
+      </c>
+      <c r="I25">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F25)</f>
+        <v>-2.3381073474884033</v>
+      </c>
+      <c r="J25">
+        <f>_xll.GSL.SF.AIRY.AI(G25)</f>
+        <v>2.3607796435252848E-9</v>
+      </c>
+    </row>
+    <row r="26" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F25)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G26">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F26)</f>
+        <v>-2.3381074368953705</v>
+      </c>
+      <c r="H26">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F26)</f>
+        <v>-2.3381074666976929</v>
+      </c>
+      <c r="I26">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F26)</f>
+        <v>-2.3381074070930481</v>
+      </c>
+      <c r="J26">
+        <f>_xll.GSL.SF.AIRY.AI(G26)</f>
+        <v>-1.8536931369466938E-8</v>
+      </c>
+    </row>
+    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F26)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G27">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F27)</f>
+        <v>-2.3381074368953705</v>
+      </c>
+      <c r="H27">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F27)</f>
+        <v>-2.3381074666976929</v>
+      </c>
+      <c r="I27">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F27)</f>
+        <v>-2.3381074070930481</v>
+      </c>
+      <c r="J27">
+        <f>_xll.GSL.SF.AIRY.AI(G27)</f>
+        <v>-1.8536931369466938E-8</v>
+      </c>
+    </row>
+    <row r="28" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F27)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G28">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F28)</f>
+        <v>-2.3381074145436287</v>
+      </c>
+      <c r="H28">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F28)</f>
+        <v>-2.3381074219942093</v>
+      </c>
+      <c r="I28">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F28)</f>
+        <v>-2.3381074070930481</v>
+      </c>
+      <c r="J28">
+        <f>_xll.GSL.SF.AIRY.AI(G28)</f>
+        <v>-2.8636480207558491E-9</v>
+      </c>
+    </row>
+    <row r="29" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F28)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G29">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F29)</f>
+        <v>-2.3381074108183384</v>
+      </c>
+      <c r="H29">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F29)</f>
+        <v>-2.3381074219942093</v>
+      </c>
+      <c r="I29">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F29)</f>
+        <v>-2.3381074070930481</v>
+      </c>
+      <c r="J29">
+        <f>_xll.GSL.SF.AIRY.AI(G29)</f>
+        <v>-2.5143429039664738E-10</v>
+      </c>
+    </row>
+    <row r="30" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F29)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G30">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F30)</f>
+        <v>-2.3381074089556932</v>
+      </c>
+      <c r="H30">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F30)</f>
+        <v>-2.3381074108183384</v>
+      </c>
+      <c r="I30">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F30)</f>
+        <v>-2.3381074070930481</v>
+      </c>
+      <c r="J30">
+        <f>_xll.GSL.SF.AIRY.AI(G30)</f>
+        <v>1.0546729787048042E-9</v>
+      </c>
+    </row>
+    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F30)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G31">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F31)</f>
+        <v>-2.3381074089556932</v>
+      </c>
+      <c r="H31">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F31)</f>
+        <v>-2.3381074108183384</v>
+      </c>
+      <c r="I31">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F31)</f>
+        <v>-2.3381074070930481</v>
+      </c>
+      <c r="J31">
+        <f>_xll.GSL.SF.AIRY.AI(G31)</f>
+        <v>1.0546729787048042E-9</v>
+      </c>
+    </row>
+    <row r="32" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F31)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G32">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F32)</f>
+        <v>-2.3381074098870158</v>
+      </c>
+      <c r="H32">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F32)</f>
+        <v>-2.3381074108183384</v>
+      </c>
+      <c r="I32">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F32)</f>
+        <v>-2.3381074089556932</v>
+      </c>
+      <c r="J32">
+        <f>_xll.GSL.SF.AIRY.AI(G32)</f>
+        <v>4.0161924329683145E-10</v>
+      </c>
+    </row>
+    <row r="33" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F32)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G33">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F33)</f>
+        <v>-2.3381074105855078</v>
+      </c>
+      <c r="H33">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F33)</f>
+        <v>-2.3381074108183384</v>
+      </c>
+      <c r="I33">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F33)</f>
+        <v>-2.3381074103526771</v>
+      </c>
+      <c r="J33">
+        <f>_xll.GSL.SF.AIRY.AI(G33)</f>
+        <v>-8.8170755791370704E-11</v>
+      </c>
+    </row>
+    <row r="34" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F33)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G34">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F34)</f>
+        <v>-2.3381074104690924</v>
+      </c>
+      <c r="H34">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F34)</f>
+        <v>-2.3381074105855078</v>
+      </c>
+      <c r="I34">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F34)</f>
+        <v>-2.3381074103526771</v>
+      </c>
+      <c r="J34">
+        <f>_xll.GSL.SF.AIRY.AI(G34)</f>
+        <v>-6.5391900771224269E-12</v>
+      </c>
+    </row>
+    <row r="35" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F34)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G35">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F35)</f>
+        <v>-2.3381074104690924</v>
+      </c>
+      <c r="H35">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F35)</f>
+        <v>-2.3381074105855078</v>
+      </c>
+      <c r="I35">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F35)</f>
+        <v>-2.3381074103526771</v>
+      </c>
+      <c r="J35">
+        <f>_xll.GSL.SF.AIRY.AI(G35)</f>
+        <v>-6.5391900771224269E-12</v>
+      </c>
+    </row>
+    <row r="36" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F35)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G36">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F36)</f>
+        <v>-2.3381074104108848</v>
+      </c>
+      <c r="H36">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F36)</f>
+        <v>-2.3381074104690924</v>
+      </c>
+      <c r="I36">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F36)</f>
+        <v>-2.3381074103526771</v>
+      </c>
+      <c r="J36">
+        <f>_xll.GSL.SF.AIRY.AI(G36)</f>
+        <v>3.4276794372001605E-11</v>
+      </c>
+    </row>
+    <row r="37" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F36)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G37">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F37)</f>
+        <v>-2.3381074104399886</v>
+      </c>
+      <c r="H37">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F37)</f>
+        <v>-2.3381074104690924</v>
+      </c>
+      <c r="I37">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F37)</f>
+        <v>-2.3381074104399886</v>
+      </c>
+      <c r="J37">
+        <f>_xll.GSL.SF.AIRY.AI(G37)</f>
+        <v>1.3868902943018387E-11</v>
+      </c>
+    </row>
+    <row r="38" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F37)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G38">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F38)</f>
+        <v>-2.3381074104618165</v>
+      </c>
+      <c r="H38">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F38)</f>
+        <v>-2.3381074104690924</v>
+      </c>
+      <c r="I38">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F38)</f>
+        <v>-2.3381074104545405</v>
+      </c>
+      <c r="J38">
+        <f>_xll.GSL.SF.AIRY.AI(G38)</f>
+        <v>-1.4371164242790251E-12</v>
+      </c>
+    </row>
+    <row r="39" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F38)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G39">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F39)</f>
+        <v>-2.3381074104581785</v>
+      </c>
+      <c r="H39">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F39)</f>
+        <v>-2.3381074104618165</v>
+      </c>
+      <c r="I39">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F39)</f>
+        <v>-2.3381074104545405</v>
+      </c>
+      <c r="J39">
+        <f>_xll.GSL.SF.AIRY.AI(G39)</f>
+        <v>1.1138196065065366E-12</v>
+      </c>
+    </row>
+    <row r="40" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F39)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G40">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F40)</f>
+        <v>-2.3381074104581785</v>
+      </c>
+      <c r="H40">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F40)</f>
+        <v>-2.3381074104618165</v>
+      </c>
+      <c r="I40">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F40)</f>
+        <v>-2.3381074104545405</v>
+      </c>
+      <c r="J40">
+        <f>_xll.GSL.SF.AIRY.AI(G40)</f>
+        <v>1.1138196065065366E-12</v>
+      </c>
+    </row>
+    <row r="41" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F40)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G41">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F41)</f>
+        <v>-2.338107410459088</v>
+      </c>
+      <c r="H41">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F41)</f>
+        <v>-2.3381074104618165</v>
+      </c>
+      <c r="I41">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F41)</f>
+        <v>-2.3381074104581785</v>
+      </c>
+      <c r="J41">
+        <f>_xll.GSL.SF.AIRY.AI(G41)</f>
+        <v>4.761863944489294E-13</v>
+      </c>
+    </row>
+    <row r="42" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F41)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G42">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F42)</f>
+        <v>-2.3381074104595427</v>
+      </c>
+      <c r="H42">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F42)</f>
+        <v>-2.3381074104599975</v>
+      </c>
+      <c r="I42">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F42)</f>
+        <v>-2.338107410459088</v>
+      </c>
+      <c r="J42">
+        <f>_xll.GSL.SF.AIRY.AI(G42)</f>
+        <v>1.5726899278121042E-13</v>
+      </c>
+    </row>
+    <row r="43" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F42)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G43">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F43)</f>
+        <v>-2.3381074104597701</v>
+      </c>
+      <c r="H43">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F43)</f>
+        <v>-2.3381074104599975</v>
+      </c>
+      <c r="I43">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F43)</f>
+        <v>-2.3381074104595427</v>
+      </c>
+      <c r="J43">
+        <f>_xll.GSL.SF.AIRY.AI(G43)</f>
+        <v>-2.1897080526380579E-15</v>
+      </c>
+    </row>
+    <row r="44" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F43)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G44">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F44)</f>
+        <v>-2.3381074104597701</v>
+      </c>
+      <c r="H44">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F44)</f>
+        <v>-2.3381074104597701</v>
+      </c>
+      <c r="I44">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F44)</f>
+        <v>-2.3381074104595427</v>
+      </c>
+      <c r="J44">
+        <f>_xll.GSL.SF.AIRY.AI(G44)</f>
+        <v>-2.1897080526380579E-15</v>
+      </c>
+    </row>
+    <row r="45" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F44)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G45">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F45)</f>
+        <v>-2.3381074104597133</v>
+      </c>
+      <c r="H45">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F45)</f>
+        <v>-2.3381074104597701</v>
+      </c>
+      <c r="I45">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F45)</f>
+        <v>-2.3381074104595427</v>
+      </c>
+      <c r="J45">
+        <f>_xll.GSL.SF.AIRY.AI(G45)</f>
+        <v>3.75237736973842E-14</v>
+      </c>
+    </row>
+    <row r="46" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F45)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G46">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F46)</f>
+        <v>-2.3381074104597417</v>
+      </c>
+      <c r="H46">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F46)</f>
+        <v>-2.3381074104597701</v>
+      </c>
+      <c r="I46">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F46)</f>
+        <v>-2.3381074104596564</v>
+      </c>
+      <c r="J46">
+        <f>_xll.GSL.SF.AIRY.AI(G46)</f>
+        <v>1.7566237183413565E-14</v>
+      </c>
+    </row>
+    <row r="47" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F46)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G47">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F47)</f>
+        <v>-2.3381074104597559</v>
+      </c>
+      <c r="H47">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F47)</f>
+        <v>-2.3381074104597701</v>
+      </c>
+      <c r="I47">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F47)</f>
+        <v>-2.3381074104597417</v>
+      </c>
+      <c r="J47">
+        <f>_xll.GSL.SF.AIRY.AI(G47)</f>
+        <v>7.6882645653877401E-15</v>
+      </c>
+    </row>
+    <row r="48" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F47)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G48">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F48)</f>
+        <v>-2.338107410459763</v>
+      </c>
+      <c r="H48">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F48)</f>
+        <v>-2.3381074104597701</v>
+      </c>
+      <c r="I48">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F48)</f>
+        <v>-2.3381074104597417</v>
+      </c>
+      <c r="J48">
+        <f>_xll.GSL.SF.AIRY.AI(G48)</f>
+        <v>2.8500738953342848E-15</v>
+      </c>
+    </row>
+    <row r="49" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F48)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G49">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F49)</f>
+        <v>-2.3381074104597666</v>
+      </c>
+      <c r="H49">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F49)</f>
+        <v>-2.3381074104597701</v>
+      </c>
+      <c r="I49">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F49)</f>
+        <v>-2.3381074104597559</v>
+      </c>
+      <c r="J49">
+        <f>_xll.GSL.SF.AIRY.AI(G49)</f>
+        <v>4.3097856030755943E-16</v>
+      </c>
+    </row>
+    <row r="50" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F49)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G50">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F50)</f>
+        <v>-2.3381074104597683</v>
+      </c>
+      <c r="H50">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F50)</f>
+        <v>-2.3381074104597701</v>
+      </c>
+      <c r="I50">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F50)</f>
+        <v>-2.3381074104597666</v>
+      </c>
+      <c r="J50">
+        <f>_xll.GSL.SF.AIRY.AI(G50)</f>
+        <v>-9.8016038512469629E-16</v>
+      </c>
+    </row>
+    <row r="51" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F50)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G51">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F51)</f>
+        <v>-2.3381074104597674</v>
+      </c>
+      <c r="H51">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F51)</f>
+        <v>-2.3381074104597683</v>
+      </c>
+      <c r="I51">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F51)</f>
+        <v>-2.3381074104597666</v>
+      </c>
+      <c r="J51">
+        <f>_xll.GSL.SF.AIRY.AI(G51)</f>
+        <v>-3.7538655136801532E-16</v>
+      </c>
+    </row>
+    <row r="52" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f>_xll.GSL.ROOT.FSOLVER.ITERATE(F51)</f>
+        <v>7.5038813227727042E-212</v>
+      </c>
+      <c r="G52">
+        <f>_xll.GSL.ROOT.FSOLVER.ROOT(F52)</f>
+        <v>-2.3381074104597674</v>
+      </c>
+      <c r="H52">
+        <f>_xll.GSL.ROOT.FSOLVER.X.LOWER(F52)</f>
+        <v>-2.3381074104597683</v>
+      </c>
+      <c r="I52">
+        <f>_xll.GSL.ROOT.FSOLVER.X.UPPER(F52)</f>
+        <v>-2.3381074104597666</v>
+      </c>
+      <c r="J52">
+        <f>_xll.GSL.SF.AIRY.AI(G52)</f>
+        <v>-3.7538655136801532E-16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>-3</v>
+      </c>
+      <c r="C3">
+        <f>_xll.GSL.SF.AIRY.AI(B3)</f>
+        <v>-0.37881429367765823</v>
+      </c>
+      <c r="D3">
+        <f>_xll.GSL_ROOT_FDFSOLVER_NEWTON()</f>
+        <v>7.1482134591343954E+119</v>
+      </c>
+      <c r="E3">
+        <f>_xll.GSL.ROOT.FDFSOLVER(D3)</f>
+        <v>5.4124369296643602E-211</v>
+      </c>
+      <c r="F3">
+        <f>_xll.GSL.ROOT.FDFSOLVER.SET(E3, _xll.XLL.FUNCTION.REGID(_xll.GSL.SF.AIRY.AI), _xll.XLL.FUNCTION.REGID(_xll.GSL.SF.AIRY.AI.DERIV), B3)</f>
+        <v>5.4124369296643602E-211</v>
+      </c>
+      <c r="G3">
+        <f>_xll.GSL.ROOT.FDFSOLVER.ROOT(F3)</f>
+        <v>-3</v>
+      </c>
+      <c r="H3">
+        <f>_xll.GSL.SF.AIRY.AI(G3)</f>
+        <v>-0.37881429367765823</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>-2</v>
+      </c>
+      <c r="C4">
+        <f>_xll.GSL.SF.AIRY.AI(B4)</f>
+        <v>0.22740742820168561</v>
+      </c>
+      <c r="F4">
+        <f>_xll.GSL.ROOT.FDFSOLVER.ITERATE(F3)</f>
+        <v>5.4124369296643602E-211</v>
+      </c>
+      <c r="G4">
+        <f>_xll.GSL.ROOT.FDFSOLVER.ROOT(F4)</f>
+        <v>-1.7958237813062898</v>
+      </c>
+      <c r="H4">
+        <f>_xll.GSL.SF.AIRY.AI(G4)</f>
+        <v>0.34288606493088997</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f>_xll.GSL.ROOT.FDFSOLVER.ITERATE(F4)</f>
+        <v>5.4124369296643602E-211</v>
+      </c>
+      <c r="G5">
+        <f>_xll.GSL.ROOT.FDFSOLVER.ROOT(F5)</f>
+        <v>-2.4715531547913008</v>
+      </c>
+      <c r="H5">
+        <f>_xll.GSL.SF.AIRY.AI(G5)</f>
+        <v>-9.2907152524821027E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f>_xll.GSL.ROOT.FDFSOLVER.ITERATE(F5)</f>
+        <v>5.4124369296643602E-211</v>
+      </c>
+      <c r="G6">
+        <f>_xll.GSL.ROOT.FDFSOLVER.ROOT(F6)</f>
+        <v>-2.3381074163730995</v>
+      </c>
+      <c r="H6">
+        <f>_xll.GSL.SF.AIRY.AI(G6)</f>
+        <v>-4.1464926628912064E-9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f>_xll.GSL.ROOT.FDFSOLVER.ITERATE(F6)</f>
+        <v>5.4124369296643602E-211</v>
+      </c>
+      <c r="G7">
+        <f>_xll.GSL.ROOT.FDFSOLVER.ROOT(F7)</f>
+        <v>-2.338107410459767</v>
+      </c>
+      <c r="H7">
+        <f>_xll.GSL.SF.AIRY.AI(G7)</f>
+        <v>2.7796004469772019E-17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f>_xll.GSL.ROOT.FDFSOLVER.ITERATE(F7)</f>
+        <v>5.4124369296643602E-211</v>
+      </c>
+      <c r="G8">
+        <f>_xll.GSL.ROOT.FDFSOLVER.ROOT(F8)</f>
+        <v>-2.338107410459767</v>
+      </c>
+      <c r="H8">
+        <f>_xll.GSL.SF.AIRY.AI(G8)</f>
+        <v>2.7796004469772019E-17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>